<commit_message>
add R history and R workspace
</commit_message>
<xml_diff>
--- a/genes_down_all_time_points_intersection.xlsx
+++ b/genes_down_all_time_points_intersection.xlsx
@@ -62,571 +62,571 @@
     <t>HD6_6H</t>
   </si>
   <si>
-    <t>428</t>
-  </si>
-  <si>
-    <t>517</t>
-  </si>
-  <si>
-    <t>1062</t>
-  </si>
-  <si>
-    <t>1417</t>
-  </si>
-  <si>
-    <t>1555</t>
-  </si>
-  <si>
-    <t>2034</t>
-  </si>
-  <si>
-    <t>2288</t>
-  </si>
-  <si>
-    <t>2321</t>
-  </si>
-  <si>
-    <t>2747</t>
-  </si>
-  <si>
-    <t>2813</t>
-  </si>
-  <si>
-    <t>3704</t>
-  </si>
-  <si>
-    <t>3707</t>
-  </si>
-  <si>
-    <t>4376</t>
-  </si>
-  <si>
-    <t>4378</t>
-  </si>
-  <si>
-    <t>4439</t>
-  </si>
-  <si>
-    <t>4629</t>
-  </si>
-  <si>
-    <t>4789</t>
-  </si>
-  <si>
-    <t>4978</t>
-  </si>
-  <si>
-    <t>5173</t>
-  </si>
-  <si>
-    <t>5317</t>
-  </si>
-  <si>
-    <t>7729</t>
-  </si>
-  <si>
-    <t>8989</t>
-  </si>
-  <si>
-    <t>9373</t>
-  </si>
-  <si>
-    <t>9393</t>
-  </si>
-  <si>
-    <t>9825</t>
-  </si>
-  <si>
-    <t>10082</t>
-  </si>
-  <si>
-    <t>10130</t>
-  </si>
-  <si>
-    <t>10530</t>
-  </si>
-  <si>
-    <t>12065</t>
-  </si>
-  <si>
-    <t>12445</t>
-  </si>
-  <si>
-    <t>12712</t>
-  </si>
-  <si>
-    <t>12740</t>
-  </si>
-  <si>
-    <t>13418</t>
-  </si>
-  <si>
-    <t>14322</t>
-  </si>
-  <si>
-    <t>15337</t>
-  </si>
-  <si>
-    <t>17608</t>
-  </si>
-  <si>
-    <t>17627</t>
-  </si>
-  <si>
-    <t>17631</t>
-  </si>
-  <si>
-    <t>17815</t>
-  </si>
-  <si>
-    <t>17820</t>
-  </si>
-  <si>
-    <t>19201</t>
-  </si>
-  <si>
-    <t>19418</t>
-  </si>
-  <si>
-    <t>19797</t>
-  </si>
-  <si>
-    <t>20341</t>
-  </si>
-  <si>
-    <t>20628</t>
-  </si>
-  <si>
-    <t>20646</t>
-  </si>
-  <si>
-    <t>20787</t>
-  </si>
-  <si>
-    <t>21055</t>
-  </si>
-  <si>
-    <t>21170</t>
-  </si>
-  <si>
-    <t>21263</t>
-  </si>
-  <si>
-    <t>21324</t>
-  </si>
-  <si>
-    <t>21404</t>
-  </si>
-  <si>
-    <t>21423</t>
-  </si>
-  <si>
-    <t>21571</t>
-  </si>
-  <si>
-    <t>21643</t>
-  </si>
-  <si>
-    <t>21853</t>
-  </si>
-  <si>
-    <t>22356</t>
-  </si>
-  <si>
-    <t>22886</t>
-  </si>
-  <si>
-    <t>23431</t>
-  </si>
-  <si>
-    <t>23706</t>
-  </si>
-  <si>
-    <t>24490</t>
-  </si>
-  <si>
-    <t>25292</t>
-  </si>
-  <si>
-    <t>25495</t>
-  </si>
-  <si>
-    <t>25595</t>
-  </si>
-  <si>
-    <t>26046</t>
-  </si>
-  <si>
-    <t>26501</t>
-  </si>
-  <si>
-    <t>26560</t>
-  </si>
-  <si>
-    <t>26802</t>
-  </si>
-  <si>
-    <t>27137</t>
-  </si>
-  <si>
-    <t>27407</t>
-  </si>
-  <si>
-    <t>27507</t>
-  </si>
-  <si>
-    <t>27592</t>
-  </si>
-  <si>
-    <t>27754</t>
-  </si>
-  <si>
-    <t>27860</t>
-  </si>
-  <si>
-    <t>28171</t>
-  </si>
-  <si>
-    <t>28412</t>
-  </si>
-  <si>
-    <t>28588</t>
-  </si>
-  <si>
-    <t>28699</t>
-  </si>
-  <si>
-    <t>28700</t>
-  </si>
-  <si>
-    <t>28776</t>
-  </si>
-  <si>
-    <t>29275</t>
-  </si>
-  <si>
-    <t>29434</t>
-  </si>
-  <si>
-    <t>30137</t>
-  </si>
-  <si>
-    <t>30215</t>
-  </si>
-  <si>
-    <t>30265</t>
-  </si>
-  <si>
-    <t>30278</t>
-  </si>
-  <si>
-    <t>30300</t>
-  </si>
-  <si>
-    <t>30345</t>
-  </si>
-  <si>
-    <t>30416</t>
-  </si>
-  <si>
-    <t>30480</t>
-  </si>
-  <si>
-    <t>30588</t>
-  </si>
-  <si>
-    <t>30619</t>
-  </si>
-  <si>
-    <t>30647</t>
-  </si>
-  <si>
-    <t>30657</t>
-  </si>
-  <si>
-    <t>30681</t>
-  </si>
-  <si>
-    <t>31005</t>
-  </si>
-  <si>
-    <t>31095</t>
-  </si>
-  <si>
-    <t>31786</t>
-  </si>
-  <si>
-    <t>31981</t>
-  </si>
-  <si>
-    <t>32157</t>
-  </si>
-  <si>
-    <t>32220</t>
-  </si>
-  <si>
-    <t>32343</t>
-  </si>
-  <si>
-    <t>33837</t>
-  </si>
-  <si>
-    <t>34008</t>
-  </si>
-  <si>
-    <t>34066</t>
-  </si>
-  <si>
-    <t>34592</t>
-  </si>
-  <si>
-    <t>34625</t>
-  </si>
-  <si>
-    <t>34646</t>
-  </si>
-  <si>
-    <t>34712</t>
-  </si>
-  <si>
-    <t>34782</t>
-  </si>
-  <si>
-    <t>36822</t>
-  </si>
-  <si>
-    <t>37183</t>
-  </si>
-  <si>
-    <t>37768</t>
-  </si>
-  <si>
-    <t>37782</t>
-  </si>
-  <si>
-    <t>37788</t>
-  </si>
-  <si>
-    <t>38972</t>
-  </si>
-  <si>
-    <t>39046</t>
-  </si>
-  <si>
-    <t>39091</t>
-  </si>
-  <si>
-    <t>40136</t>
-  </si>
-  <si>
-    <t>40210</t>
-  </si>
-  <si>
-    <t>40314</t>
-  </si>
-  <si>
-    <t>40408</t>
-  </si>
-  <si>
-    <t>40481</t>
-  </si>
-  <si>
-    <t>40591</t>
-  </si>
-  <si>
-    <t>40645</t>
-  </si>
-  <si>
-    <t>41061</t>
-  </si>
-  <si>
-    <t>41182</t>
-  </si>
-  <si>
-    <t>41780</t>
-  </si>
-  <si>
-    <t>41833</t>
-  </si>
-  <si>
-    <t>41840</t>
-  </si>
-  <si>
-    <t>41893</t>
-  </si>
-  <si>
-    <t>42068</t>
-  </si>
-  <si>
-    <t>42399</t>
-  </si>
-  <si>
-    <t>42449</t>
-  </si>
-  <si>
-    <t>42694</t>
-  </si>
-  <si>
-    <t>42705</t>
-  </si>
-  <si>
-    <t>43222</t>
-  </si>
-  <si>
-    <t>43677</t>
-  </si>
-  <si>
-    <t>43771</t>
-  </si>
-  <si>
-    <t>46630</t>
-  </si>
-  <si>
-    <t>48902</t>
-  </si>
-  <si>
-    <t>49098</t>
-  </si>
-  <si>
-    <t>50036</t>
-  </si>
-  <si>
-    <t>50051</t>
-  </si>
-  <si>
-    <t>50055</t>
-  </si>
-  <si>
-    <t>50948</t>
-  </si>
-  <si>
-    <t>50957</t>
-  </si>
-  <si>
-    <t>51056</t>
-  </si>
-  <si>
-    <t>51082</t>
-  </si>
-  <si>
-    <t>51626</t>
-  </si>
-  <si>
-    <t>51711</t>
-  </si>
-  <si>
-    <t>51764</t>
-  </si>
-  <si>
-    <t>52140</t>
-  </si>
-  <si>
-    <t>52170</t>
-  </si>
-  <si>
-    <t>52585</t>
-  </si>
-  <si>
-    <t>52749</t>
-  </si>
-  <si>
-    <t>52894</t>
-  </si>
-  <si>
-    <t>53004</t>
-  </si>
-  <si>
-    <t>53039</t>
-  </si>
-  <si>
-    <t>53224</t>
-  </si>
-  <si>
-    <t>53681</t>
-  </si>
-  <si>
-    <t>53730</t>
-  </si>
-  <si>
-    <t>53875</t>
-  </si>
-  <si>
-    <t>53969</t>
-  </si>
-  <si>
-    <t>53979</t>
-  </si>
-  <si>
-    <t>54108</t>
-  </si>
-  <si>
-    <t>54810</t>
-  </si>
-  <si>
-    <t>54843</t>
-  </si>
-  <si>
-    <t>55204</t>
-  </si>
-  <si>
-    <t>55216</t>
-  </si>
-  <si>
-    <t>55250</t>
-  </si>
-  <si>
-    <t>55707</t>
-  </si>
-  <si>
-    <t>55845</t>
-  </si>
-  <si>
-    <t>55928</t>
-  </si>
-  <si>
-    <t>55960</t>
-  </si>
-  <si>
-    <t>55995</t>
-  </si>
-  <si>
-    <t>56028</t>
-  </si>
-  <si>
-    <t>56131</t>
-  </si>
-  <si>
-    <t>56186</t>
-  </si>
-  <si>
-    <t>56197</t>
-  </si>
-  <si>
-    <t>56226</t>
-  </si>
-  <si>
-    <t>56317</t>
-  </si>
-  <si>
-    <t>56407</t>
-  </si>
-  <si>
-    <t>56422</t>
-  </si>
-  <si>
-    <t>56491</t>
-  </si>
-  <si>
-    <t>56500</t>
-  </si>
-  <si>
-    <t>AC004233.3</t>
+    <t>430</t>
+  </si>
+  <si>
+    <t>520</t>
+  </si>
+  <si>
+    <t>1067</t>
+  </si>
+  <si>
+    <t>1420</t>
+  </si>
+  <si>
+    <t>1556</t>
+  </si>
+  <si>
+    <t>2032</t>
+  </si>
+  <si>
+    <t>2285</t>
+  </si>
+  <si>
+    <t>2319</t>
+  </si>
+  <si>
+    <t>2743</t>
+  </si>
+  <si>
+    <t>2809</t>
+  </si>
+  <si>
+    <t>3702</t>
+  </si>
+  <si>
+    <t>3705</t>
+  </si>
+  <si>
+    <t>4369</t>
+  </si>
+  <si>
+    <t>4371</t>
+  </si>
+  <si>
+    <t>4432</t>
+  </si>
+  <si>
+    <t>4622</t>
+  </si>
+  <si>
+    <t>4784</t>
+  </si>
+  <si>
+    <t>4968</t>
+  </si>
+  <si>
+    <t>5164</t>
+  </si>
+  <si>
+    <t>5309</t>
+  </si>
+  <si>
+    <t>7715</t>
+  </si>
+  <si>
+    <t>8971</t>
+  </si>
+  <si>
+    <t>9354</t>
+  </si>
+  <si>
+    <t>9374</t>
+  </si>
+  <si>
+    <t>9799</t>
+  </si>
+  <si>
+    <t>10056</t>
+  </si>
+  <si>
+    <t>10103</t>
+  </si>
+  <si>
+    <t>10496</t>
+  </si>
+  <si>
+    <t>12406</t>
+  </si>
+  <si>
+    <t>12672</t>
+  </si>
+  <si>
+    <t>12700</t>
+  </si>
+  <si>
+    <t>13376</t>
+  </si>
+  <si>
+    <t>14279</t>
+  </si>
+  <si>
+    <t>15291</t>
+  </si>
+  <si>
+    <t>17543</t>
+  </si>
+  <si>
+    <t>17561</t>
+  </si>
+  <si>
+    <t>17565</t>
+  </si>
+  <si>
+    <t>17749</t>
+  </si>
+  <si>
+    <t>17754</t>
+  </si>
+  <si>
+    <t>19131</t>
+  </si>
+  <si>
+    <t>19348</t>
+  </si>
+  <si>
+    <t>19728</t>
+  </si>
+  <si>
+    <t>20274</t>
+  </si>
+  <si>
+    <t>20560</t>
+  </si>
+  <si>
+    <t>20578</t>
+  </si>
+  <si>
+    <t>20719</t>
+  </si>
+  <si>
+    <t>20979</t>
+  </si>
+  <si>
+    <t>21094</t>
+  </si>
+  <si>
+    <t>21186</t>
+  </si>
+  <si>
+    <t>21247</t>
+  </si>
+  <si>
+    <t>21328</t>
+  </si>
+  <si>
+    <t>21347</t>
+  </si>
+  <si>
+    <t>21495</t>
+  </si>
+  <si>
+    <t>21567</t>
+  </si>
+  <si>
+    <t>21777</t>
+  </si>
+  <si>
+    <t>22280</t>
+  </si>
+  <si>
+    <t>22810</t>
+  </si>
+  <si>
+    <t>23361</t>
+  </si>
+  <si>
+    <t>23636</t>
+  </si>
+  <si>
+    <t>24423</t>
+  </si>
+  <si>
+    <t>25231</t>
+  </si>
+  <si>
+    <t>25451</t>
+  </si>
+  <si>
+    <t>25574</t>
+  </si>
+  <si>
+    <t>26048</t>
+  </si>
+  <si>
+    <t>26495</t>
+  </si>
+  <si>
+    <t>26553</t>
+  </si>
+  <si>
+    <t>26797</t>
+  </si>
+  <si>
+    <t>27132</t>
+  </si>
+  <si>
+    <t>27400</t>
+  </si>
+  <si>
+    <t>27500</t>
+  </si>
+  <si>
+    <t>27585</t>
+  </si>
+  <si>
+    <t>27746</t>
+  </si>
+  <si>
+    <t>27851</t>
+  </si>
+  <si>
+    <t>28161</t>
+  </si>
+  <si>
+    <t>28401</t>
+  </si>
+  <si>
+    <t>28577</t>
+  </si>
+  <si>
+    <t>28688</t>
+  </si>
+  <si>
+    <t>28689</t>
+  </si>
+  <si>
+    <t>28729</t>
+  </si>
+  <si>
+    <t>28762</t>
+  </si>
+  <si>
+    <t>29258</t>
+  </si>
+  <si>
+    <t>29417</t>
+  </si>
+  <si>
+    <t>30120</t>
+  </si>
+  <si>
+    <t>30198</t>
+  </si>
+  <si>
+    <t>30249</t>
+  </si>
+  <si>
+    <t>30262</t>
+  </si>
+  <si>
+    <t>30284</t>
+  </si>
+  <si>
+    <t>30329</t>
+  </si>
+  <si>
+    <t>30400</t>
+  </si>
+  <si>
+    <t>30461</t>
+  </si>
+  <si>
+    <t>30569</t>
+  </si>
+  <si>
+    <t>30600</t>
+  </si>
+  <si>
+    <t>30628</t>
+  </si>
+  <si>
+    <t>30638</t>
+  </si>
+  <si>
+    <t>30662</t>
+  </si>
+  <si>
+    <t>30983</t>
+  </si>
+  <si>
+    <t>31073</t>
+  </si>
+  <si>
+    <t>31764</t>
+  </si>
+  <si>
+    <t>31959</t>
+  </si>
+  <si>
+    <t>32135</t>
+  </si>
+  <si>
+    <t>32197</t>
+  </si>
+  <si>
+    <t>32319</t>
+  </si>
+  <si>
+    <t>33827</t>
+  </si>
+  <si>
+    <t>34000</t>
+  </si>
+  <si>
+    <t>34057</t>
+  </si>
+  <si>
+    <t>34584</t>
+  </si>
+  <si>
+    <t>34617</t>
+  </si>
+  <si>
+    <t>34638</t>
+  </si>
+  <si>
+    <t>34704</t>
+  </si>
+  <si>
+    <t>34774</t>
+  </si>
+  <si>
+    <t>36814</t>
+  </si>
+  <si>
+    <t>37175</t>
+  </si>
+  <si>
+    <t>37760</t>
+  </si>
+  <si>
+    <t>37774</t>
+  </si>
+  <si>
+    <t>37780</t>
+  </si>
+  <si>
+    <t>38965</t>
+  </si>
+  <si>
+    <t>39039</t>
+  </si>
+  <si>
+    <t>39083</t>
+  </si>
+  <si>
+    <t>40123</t>
+  </si>
+  <si>
+    <t>40197</t>
+  </si>
+  <si>
+    <t>40301</t>
+  </si>
+  <si>
+    <t>40395</t>
+  </si>
+  <si>
+    <t>40468</t>
+  </si>
+  <si>
+    <t>40578</t>
+  </si>
+  <si>
+    <t>40632</t>
+  </si>
+  <si>
+    <t>41049</t>
+  </si>
+  <si>
+    <t>41170</t>
+  </si>
+  <si>
+    <t>41774</t>
+  </si>
+  <si>
+    <t>41827</t>
+  </si>
+  <si>
+    <t>41834</t>
+  </si>
+  <si>
+    <t>41887</t>
+  </si>
+  <si>
+    <t>42063</t>
+  </si>
+  <si>
+    <t>42393</t>
+  </si>
+  <si>
+    <t>42443</t>
+  </si>
+  <si>
+    <t>42687</t>
+  </si>
+  <si>
+    <t>42698</t>
+  </si>
+  <si>
+    <t>43216</t>
+  </si>
+  <si>
+    <t>43670</t>
+  </si>
+  <si>
+    <t>43765</t>
+  </si>
+  <si>
+    <t>46623</t>
+  </si>
+  <si>
+    <t>48894</t>
+  </si>
+  <si>
+    <t>49090</t>
+  </si>
+  <si>
+    <t>50025</t>
+  </si>
+  <si>
+    <t>50040</t>
+  </si>
+  <si>
+    <t>50044</t>
+  </si>
+  <si>
+    <t>50941</t>
+  </si>
+  <si>
+    <t>50950</t>
+  </si>
+  <si>
+    <t>51049</t>
+  </si>
+  <si>
+    <t>51075</t>
+  </si>
+  <si>
+    <t>51616</t>
+  </si>
+  <si>
+    <t>51703</t>
+  </si>
+  <si>
+    <t>51756</t>
+  </si>
+  <si>
+    <t>52137</t>
+  </si>
+  <si>
+    <t>52167</t>
+  </si>
+  <si>
+    <t>52583</t>
+  </si>
+  <si>
+    <t>52746</t>
+  </si>
+  <si>
+    <t>52890</t>
+  </si>
+  <si>
+    <t>52999</t>
+  </si>
+  <si>
+    <t>53034</t>
+  </si>
+  <si>
+    <t>53220</t>
+  </si>
+  <si>
+    <t>53677</t>
+  </si>
+  <si>
+    <t>53726</t>
+  </si>
+  <si>
+    <t>53871</t>
+  </si>
+  <si>
+    <t>53965</t>
+  </si>
+  <si>
+    <t>53975</t>
+  </si>
+  <si>
+    <t>54104</t>
+  </si>
+  <si>
+    <t>54806</t>
+  </si>
+  <si>
+    <t>54839</t>
+  </si>
+  <si>
+    <t>55200</t>
+  </si>
+  <si>
+    <t>55212</t>
+  </si>
+  <si>
+    <t>55246</t>
+  </si>
+  <si>
+    <t>55705</t>
+  </si>
+  <si>
+    <t>55844</t>
+  </si>
+  <si>
+    <t>55927</t>
+  </si>
+  <si>
+    <t>55959</t>
+  </si>
+  <si>
+    <t>55994</t>
+  </si>
+  <si>
+    <t>56027</t>
+  </si>
+  <si>
+    <t>56129</t>
+  </si>
+  <si>
+    <t>56184</t>
+  </si>
+  <si>
+    <t>56195</t>
+  </si>
+  <si>
+    <t>56224</t>
+  </si>
+  <si>
+    <t>56315</t>
+  </si>
+  <si>
+    <t>56405</t>
+  </si>
+  <si>
+    <t>56420</t>
+  </si>
+  <si>
+    <t>56489</t>
+  </si>
+  <si>
+    <t>56498</t>
+  </si>
+  <si>
+    <t>AC004233.2</t>
   </si>
   <si>
     <t>AC004706.1</t>
   </si>
   <si>
-    <t>AC005840.4</t>
+    <t>AC005840.5</t>
   </si>
   <si>
     <t>AC007000.1</t>
@@ -704,9 +704,6 @@
     <t>AC114490.1</t>
   </si>
   <si>
-    <t>AC239868.1</t>
-  </si>
-  <si>
     <t>ACSM3</t>
   </si>
   <si>
@@ -855,6 +852,9 @@
   </si>
   <si>
     <t>HIST1H2BF</t>
+  </si>
+  <si>
+    <t>HIST2H2BC</t>
   </si>
   <si>
     <t>HLA-DPA1</t>
@@ -2769,49 +2769,49 @@
         <v>230</v>
       </c>
       <c r="C30" t="n">
-        <v>267.0</v>
+        <v>48.0</v>
       </c>
       <c r="D30" t="n">
-        <v>277.0</v>
+        <v>29.0</v>
       </c>
       <c r="E30" t="n">
-        <v>289.0</v>
+        <v>13.0</v>
       </c>
       <c r="F30" t="n">
-        <v>182.0</v>
+        <v>13.0</v>
       </c>
       <c r="G30" t="n">
-        <v>193.0</v>
+        <v>26.0</v>
       </c>
       <c r="H30" t="n">
-        <v>80.0</v>
+        <v>4.0</v>
       </c>
       <c r="I30" t="n">
-        <v>219.0</v>
+        <v>26.0</v>
       </c>
       <c r="J30" t="n">
-        <v>194.0</v>
+        <v>14.0</v>
       </c>
       <c r="K30" t="n">
-        <v>58.0</v>
+        <v>8.0</v>
       </c>
       <c r="L30" t="n">
-        <v>110.0</v>
+        <v>12.0</v>
       </c>
       <c r="M30" t="n">
-        <v>120.0</v>
+        <v>8.0</v>
       </c>
       <c r="N30" t="n">
-        <v>87.0</v>
+        <v>11.0</v>
       </c>
       <c r="O30" t="n">
-        <v>111.0</v>
+        <v>9.0</v>
       </c>
       <c r="P30" t="n">
-        <v>62.0</v>
+        <v>5.0</v>
       </c>
       <c r="Q30" t="n">
-        <v>228.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="31">
@@ -2822,49 +2822,49 @@
         <v>231</v>
       </c>
       <c r="C31" t="n">
-        <v>48.0</v>
+        <v>31.0</v>
       </c>
       <c r="D31" t="n">
-        <v>29.0</v>
+        <v>33.0</v>
       </c>
       <c r="E31" t="n">
-        <v>13.0</v>
+        <v>23.0</v>
       </c>
       <c r="F31" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="G31" t="n">
-        <v>26.0</v>
+        <v>7.0</v>
       </c>
       <c r="H31" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="I31" t="n">
-        <v>26.0</v>
+        <v>18.0</v>
       </c>
       <c r="J31" t="n">
-        <v>14.0</v>
+        <v>9.0</v>
       </c>
       <c r="K31" t="n">
         <v>8.0</v>
       </c>
       <c r="L31" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="O31" t="n">
         <v>12.0</v>
       </c>
-      <c r="M31" t="n">
+      <c r="P31" t="n">
         <v>8.0</v>
       </c>
-      <c r="N31" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="O31" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="P31" t="n">
-        <v>5.0</v>
-      </c>
       <c r="Q31" t="n">
-        <v>20.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="32">
@@ -2875,49 +2875,49 @@
         <v>232</v>
       </c>
       <c r="C32" t="n">
-        <v>31.0</v>
+        <v>6.0</v>
       </c>
       <c r="D32" t="n">
-        <v>33.0</v>
+        <v>12.0</v>
       </c>
       <c r="E32" t="n">
-        <v>23.0</v>
+        <v>8.0</v>
       </c>
       <c r="F32" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
       <c r="G32" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="H32" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="I32" t="n">
-        <v>18.0</v>
+        <v>2.0</v>
       </c>
       <c r="J32" t="n">
-        <v>9.0</v>
+        <v>4.0</v>
       </c>
       <c r="K32" t="n">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="L32" t="n">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
       <c r="M32" t="n">
-        <v>30.0</v>
+        <v>4.0</v>
       </c>
       <c r="N32" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="O32" t="n">
-        <v>12.0</v>
+        <v>2.0</v>
       </c>
       <c r="P32" t="n">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="Q32" t="n">
-        <v>31.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="33">
@@ -2928,46 +2928,46 @@
         <v>233</v>
       </c>
       <c r="C33" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="O33" t="n">
         <v>6.0</v>
       </c>
-      <c r="D33" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="E33" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G33" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="H33" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I33" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="J33" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="K33" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="L33" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="M33" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="N33" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="O33" t="n">
-        <v>2.0</v>
-      </c>
       <c r="P33" t="n">
-        <v>2.0</v>
+        <v>16.0</v>
       </c>
       <c r="Q33" t="n">
         <v>4.0</v>
@@ -2981,49 +2981,49 @@
         <v>234</v>
       </c>
       <c r="C34" t="n">
-        <v>24.0</v>
+        <v>19.0</v>
       </c>
       <c r="D34" t="n">
-        <v>33.0</v>
+        <v>12.0</v>
       </c>
       <c r="E34" t="n">
-        <v>33.0</v>
+        <v>19.0</v>
       </c>
       <c r="F34" t="n">
-        <v>13.0</v>
+        <v>7.0</v>
       </c>
       <c r="G34" t="n">
-        <v>25.0</v>
+        <v>6.0</v>
       </c>
       <c r="H34" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="I34" t="n">
-        <v>16.0</v>
+        <v>8.0</v>
       </c>
       <c r="J34" t="n">
         <v>8.0</v>
       </c>
       <c r="K34" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="L34" t="n">
-        <v>14.0</v>
+        <v>11.0</v>
       </c>
       <c r="M34" t="n">
         <v>8.0</v>
       </c>
       <c r="N34" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="O34" t="n">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="P34" t="n">
-        <v>16.0</v>
+        <v>2.0</v>
       </c>
       <c r="Q34" t="n">
-        <v>4.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="35">
@@ -3034,49 +3034,49 @@
         <v>235</v>
       </c>
       <c r="C35" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="M35" t="n">
         <v>19.0</v>
       </c>
-      <c r="D35" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="E35" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="F35" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="G35" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="H35" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="I35" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="J35" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="K35" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="L35" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="M35" t="n">
-        <v>8.0</v>
-      </c>
       <c r="N35" t="n">
-        <v>5.0</v>
+        <v>18.0</v>
       </c>
       <c r="O35" t="n">
         <v>10.0</v>
       </c>
       <c r="P35" t="n">
-        <v>2.0</v>
+        <v>15.0</v>
       </c>
       <c r="Q35" t="n">
-        <v>27.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="36">
@@ -3087,49 +3087,49 @@
         <v>236</v>
       </c>
       <c r="C36" t="n">
-        <v>60.0</v>
+        <v>41.0</v>
       </c>
       <c r="D36" t="n">
-        <v>49.0</v>
+        <v>32.0</v>
       </c>
       <c r="E36" t="n">
-        <v>58.0</v>
+        <v>27.0</v>
       </c>
       <c r="F36" t="n">
-        <v>25.0</v>
+        <v>7.0</v>
       </c>
       <c r="G36" t="n">
-        <v>25.0</v>
+        <v>8.0</v>
       </c>
       <c r="H36" t="n">
-        <v>14.0</v>
+        <v>1.0</v>
       </c>
       <c r="I36" t="n">
-        <v>22.0</v>
+        <v>16.0</v>
       </c>
       <c r="J36" t="n">
-        <v>24.0</v>
+        <v>1.0</v>
       </c>
       <c r="K36" t="n">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="L36" t="n">
-        <v>20.0</v>
+        <v>1.0</v>
       </c>
       <c r="M36" t="n">
-        <v>19.0</v>
+        <v>0.0</v>
       </c>
       <c r="N36" t="n">
-        <v>18.0</v>
+        <v>4.0</v>
       </c>
       <c r="O36" t="n">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
       <c r="P36" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>61.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37">
@@ -3140,49 +3140,49 @@
         <v>237</v>
       </c>
       <c r="C37" t="n">
-        <v>41.0</v>
+        <v>18.0</v>
       </c>
       <c r="D37" t="n">
-        <v>32.0</v>
+        <v>13.0</v>
       </c>
       <c r="E37" t="n">
-        <v>27.0</v>
+        <v>26.0</v>
       </c>
       <c r="F37" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="G37" t="n">
-        <v>8.0</v>
+        <v>11.0</v>
       </c>
       <c r="H37" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="I37" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="O37" t="n">
         <v>16.0</v>
       </c>
-      <c r="J37" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="K37" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="L37" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="M37" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N37" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="O37" t="n">
-        <v>7.0</v>
-      </c>
       <c r="P37" t="n">
-        <v>0.0</v>
+        <v>24.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="38">
@@ -3193,49 +3193,49 @@
         <v>238</v>
       </c>
       <c r="C38" t="n">
-        <v>18.0</v>
+        <v>1936.0</v>
       </c>
       <c r="D38" t="n">
-        <v>13.0</v>
+        <v>2268.0</v>
       </c>
       <c r="E38" t="n">
-        <v>26.0</v>
+        <v>2799.0</v>
       </c>
       <c r="F38" t="n">
-        <v>9.0</v>
+        <v>1561.0</v>
       </c>
       <c r="G38" t="n">
-        <v>11.0</v>
+        <v>1875.0</v>
       </c>
       <c r="H38" t="n">
-        <v>6.0</v>
+        <v>1008.0</v>
       </c>
       <c r="I38" t="n">
-        <v>31.0</v>
+        <v>1922.0</v>
       </c>
       <c r="J38" t="n">
-        <v>13.0</v>
+        <v>1565.0</v>
       </c>
       <c r="K38" t="n">
-        <v>6.0</v>
+        <v>792.0</v>
       </c>
       <c r="L38" t="n">
-        <v>9.0</v>
+        <v>1220.0</v>
       </c>
       <c r="M38" t="n">
-        <v>20.0</v>
+        <v>2248.0</v>
       </c>
       <c r="N38" t="n">
-        <v>2.0</v>
+        <v>671.0</v>
       </c>
       <c r="O38" t="n">
-        <v>16.0</v>
+        <v>1433.0</v>
       </c>
       <c r="P38" t="n">
-        <v>24.0</v>
+        <v>1619.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>9.0</v>
+        <v>2199.0</v>
       </c>
     </row>
     <row r="39">
@@ -3246,49 +3246,49 @@
         <v>239</v>
       </c>
       <c r="C39" t="n">
-        <v>1936.0</v>
+        <v>12.0</v>
       </c>
       <c r="D39" t="n">
-        <v>2268.0</v>
+        <v>14.0</v>
       </c>
       <c r="E39" t="n">
-        <v>2799.0</v>
+        <v>9.0</v>
       </c>
       <c r="F39" t="n">
-        <v>1561.0</v>
+        <v>1.0</v>
       </c>
       <c r="G39" t="n">
-        <v>1875.0</v>
+        <v>2.0</v>
       </c>
       <c r="H39" t="n">
-        <v>1008.0</v>
+        <v>0.0</v>
       </c>
       <c r="I39" t="n">
-        <v>1922.0</v>
+        <v>8.0</v>
       </c>
       <c r="J39" t="n">
-        <v>1565.0</v>
+        <v>8.0</v>
       </c>
       <c r="K39" t="n">
-        <v>792.0</v>
+        <v>0.0</v>
       </c>
       <c r="L39" t="n">
-        <v>1220.0</v>
+        <v>6.0</v>
       </c>
       <c r="M39" t="n">
-        <v>2248.0</v>
+        <v>16.0</v>
       </c>
       <c r="N39" t="n">
-        <v>671.0</v>
+        <v>0.0</v>
       </c>
       <c r="O39" t="n">
-        <v>1433.0</v>
+        <v>10.0</v>
       </c>
       <c r="P39" t="n">
-        <v>1619.0</v>
+        <v>11.0</v>
       </c>
       <c r="Q39" t="n">
-        <v>2199.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="40">
@@ -3299,49 +3299,49 @@
         <v>240</v>
       </c>
       <c r="C40" t="n">
-        <v>12.0</v>
+        <v>1092.0</v>
       </c>
       <c r="D40" t="n">
-        <v>14.0</v>
+        <v>1091.0</v>
       </c>
       <c r="E40" t="n">
-        <v>9.0</v>
+        <v>1131.0</v>
       </c>
       <c r="F40" t="n">
-        <v>1.0</v>
+        <v>441.0</v>
       </c>
       <c r="G40" t="n">
-        <v>2.0</v>
+        <v>581.0</v>
       </c>
       <c r="H40" t="n">
-        <v>0.0</v>
+        <v>351.0</v>
       </c>
       <c r="I40" t="n">
-        <v>8.0</v>
+        <v>553.0</v>
       </c>
       <c r="J40" t="n">
-        <v>8.0</v>
+        <v>481.0</v>
       </c>
       <c r="K40" t="n">
-        <v>0.0</v>
+        <v>266.0</v>
       </c>
       <c r="L40" t="n">
-        <v>6.0</v>
+        <v>322.0</v>
       </c>
       <c r="M40" t="n">
-        <v>16.0</v>
+        <v>417.0</v>
       </c>
       <c r="N40" t="n">
-        <v>0.0</v>
+        <v>244.0</v>
       </c>
       <c r="O40" t="n">
-        <v>10.0</v>
+        <v>338.0</v>
       </c>
       <c r="P40" t="n">
-        <v>11.0</v>
+        <v>314.0</v>
       </c>
       <c r="Q40" t="n">
-        <v>7.0</v>
+        <v>1267.0</v>
       </c>
     </row>
     <row r="41">
@@ -3352,49 +3352,49 @@
         <v>241</v>
       </c>
       <c r="C41" t="n">
-        <v>1092.0</v>
+        <v>6.0</v>
       </c>
       <c r="D41" t="n">
-        <v>1091.0</v>
+        <v>14.0</v>
       </c>
       <c r="E41" t="n">
-        <v>1131.0</v>
+        <v>12.0</v>
       </c>
       <c r="F41" t="n">
-        <v>441.0</v>
+        <v>2.0</v>
       </c>
       <c r="G41" t="n">
-        <v>581.0</v>
+        <v>2.0</v>
       </c>
       <c r="H41" t="n">
-        <v>351.0</v>
+        <v>0.0</v>
       </c>
       <c r="I41" t="n">
-        <v>553.0</v>
+        <v>2.0</v>
       </c>
       <c r="J41" t="n">
-        <v>481.0</v>
+        <v>2.0</v>
       </c>
       <c r="K41" t="n">
-        <v>266.0</v>
+        <v>2.0</v>
       </c>
       <c r="L41" t="n">
-        <v>322.0</v>
+        <v>6.0</v>
       </c>
       <c r="M41" t="n">
-        <v>417.0</v>
+        <v>4.0</v>
       </c>
       <c r="N41" t="n">
-        <v>244.0</v>
+        <v>2.0</v>
       </c>
       <c r="O41" t="n">
-        <v>338.0</v>
+        <v>6.0</v>
       </c>
       <c r="P41" t="n">
-        <v>314.0</v>
+        <v>4.0</v>
       </c>
       <c r="Q41" t="n">
-        <v>1267.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="42">
@@ -3405,49 +3405,49 @@
         <v>242</v>
       </c>
       <c r="C42" t="n">
-        <v>6.0</v>
+        <v>659.0</v>
       </c>
       <c r="D42" t="n">
-        <v>14.0</v>
+        <v>758.0</v>
       </c>
       <c r="E42" t="n">
-        <v>12.0</v>
+        <v>705.0</v>
       </c>
       <c r="F42" t="n">
-        <v>2.0</v>
+        <v>426.0</v>
       </c>
       <c r="G42" t="n">
-        <v>2.0</v>
+        <v>533.0</v>
       </c>
       <c r="H42" t="n">
-        <v>0.0</v>
+        <v>281.0</v>
       </c>
       <c r="I42" t="n">
-        <v>2.0</v>
+        <v>581.0</v>
       </c>
       <c r="J42" t="n">
-        <v>2.0</v>
+        <v>439.0</v>
       </c>
       <c r="K42" t="n">
-        <v>2.0</v>
+        <v>179.0</v>
       </c>
       <c r="L42" t="n">
-        <v>6.0</v>
+        <v>359.0</v>
       </c>
       <c r="M42" t="n">
-        <v>4.0</v>
+        <v>614.0</v>
       </c>
       <c r="N42" t="n">
-        <v>2.0</v>
+        <v>280.0</v>
       </c>
       <c r="O42" t="n">
-        <v>6.0</v>
+        <v>410.0</v>
       </c>
       <c r="P42" t="n">
-        <v>4.0</v>
+        <v>473.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>3.0</v>
+        <v>701.0</v>
       </c>
     </row>
     <row r="43">
@@ -3458,49 +3458,49 @@
         <v>243</v>
       </c>
       <c r="C43" t="n">
-        <v>659.0</v>
+        <v>67.0</v>
       </c>
       <c r="D43" t="n">
-        <v>758.0</v>
+        <v>69.0</v>
       </c>
       <c r="E43" t="n">
-        <v>705.0</v>
+        <v>86.0</v>
       </c>
       <c r="F43" t="n">
-        <v>426.0</v>
+        <v>56.0</v>
       </c>
       <c r="G43" t="n">
-        <v>533.0</v>
+        <v>46.0</v>
       </c>
       <c r="H43" t="n">
-        <v>281.0</v>
+        <v>19.0</v>
       </c>
       <c r="I43" t="n">
-        <v>581.0</v>
+        <v>52.0</v>
       </c>
       <c r="J43" t="n">
-        <v>439.0</v>
+        <v>41.0</v>
       </c>
       <c r="K43" t="n">
-        <v>179.0</v>
+        <v>14.0</v>
       </c>
       <c r="L43" t="n">
-        <v>359.0</v>
+        <v>48.0</v>
       </c>
       <c r="M43" t="n">
-        <v>614.0</v>
+        <v>22.0</v>
       </c>
       <c r="N43" t="n">
-        <v>280.0</v>
+        <v>24.0</v>
       </c>
       <c r="O43" t="n">
-        <v>410.0</v>
+        <v>51.0</v>
       </c>
       <c r="P43" t="n">
-        <v>473.0</v>
+        <v>32.0</v>
       </c>
       <c r="Q43" t="n">
-        <v>701.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="44">
@@ -3511,49 +3511,49 @@
         <v>244</v>
       </c>
       <c r="C44" t="n">
-        <v>67.0</v>
+        <v>41.0</v>
       </c>
       <c r="D44" t="n">
-        <v>69.0</v>
+        <v>46.0</v>
       </c>
       <c r="E44" t="n">
-        <v>86.0</v>
+        <v>61.0</v>
       </c>
       <c r="F44" t="n">
-        <v>56.0</v>
+        <v>42.0</v>
       </c>
       <c r="G44" t="n">
-        <v>46.0</v>
+        <v>30.0</v>
       </c>
       <c r="H44" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="K44" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="M44" t="n">
         <v>19.0</v>
       </c>
-      <c r="I44" t="n">
-        <v>52.0</v>
-      </c>
-      <c r="J44" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="K44" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="L44" t="n">
-        <v>48.0</v>
-      </c>
-      <c r="M44" t="n">
-        <v>22.0</v>
-      </c>
       <c r="N44" t="n">
-        <v>24.0</v>
+        <v>6.0</v>
       </c>
       <c r="O44" t="n">
-        <v>51.0</v>
+        <v>6.0</v>
       </c>
       <c r="P44" t="n">
-        <v>32.0</v>
+        <v>15.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>49.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="45">
@@ -3564,49 +3564,49 @@
         <v>245</v>
       </c>
       <c r="C45" t="n">
-        <v>41.0</v>
+        <v>75.0</v>
       </c>
       <c r="D45" t="n">
-        <v>46.0</v>
+        <v>125.0</v>
       </c>
       <c r="E45" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>84.0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="M45" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="O45" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="P45" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="Q45" t="n">
         <v>61.0</v>
-      </c>
-      <c r="F45" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="G45" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="H45" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="I45" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="J45" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="K45" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="L45" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="M45" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="N45" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="O45" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="P45" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="Q45" t="n">
-        <v>8.0</v>
       </c>
     </row>
     <row r="46">
@@ -3617,49 +3617,49 @@
         <v>246</v>
       </c>
       <c r="C46" t="n">
-        <v>75.0</v>
+        <v>87.0</v>
       </c>
       <c r="D46" t="n">
-        <v>125.0</v>
+        <v>97.0</v>
       </c>
       <c r="E46" t="n">
-        <v>123.0</v>
+        <v>53.0</v>
       </c>
       <c r="F46" t="n">
-        <v>55.0</v>
+        <v>51.0</v>
       </c>
       <c r="G46" t="n">
-        <v>84.0</v>
+        <v>44.0</v>
       </c>
       <c r="H46" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="I46" t="n">
         <v>43.0</v>
       </c>
-      <c r="I46" t="n">
-        <v>62.0</v>
-      </c>
       <c r="J46" t="n">
-        <v>43.0</v>
+        <v>30.0</v>
       </c>
       <c r="K46" t="n">
-        <v>26.0</v>
+        <v>18.0</v>
       </c>
       <c r="L46" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="O46" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="P46" t="n">
         <v>29.0</v>
       </c>
-      <c r="M46" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="N46" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="O46" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="P46" t="n">
-        <v>30.0</v>
-      </c>
       <c r="Q46" t="n">
-        <v>61.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="47">
@@ -3670,49 +3670,49 @@
         <v>247</v>
       </c>
       <c r="C47" t="n">
-        <v>87.0</v>
+        <v>667.0</v>
       </c>
       <c r="D47" t="n">
-        <v>97.0</v>
+        <v>664.0</v>
       </c>
       <c r="E47" t="n">
-        <v>53.0</v>
+        <v>756.0</v>
       </c>
       <c r="F47" t="n">
-        <v>51.0</v>
+        <v>398.0</v>
       </c>
       <c r="G47" t="n">
-        <v>44.0</v>
+        <v>424.0</v>
       </c>
       <c r="H47" t="n">
-        <v>15.0</v>
+        <v>334.0</v>
       </c>
       <c r="I47" t="n">
-        <v>43.0</v>
+        <v>451.0</v>
       </c>
       <c r="J47" t="n">
-        <v>30.0</v>
+        <v>362.0</v>
       </c>
       <c r="K47" t="n">
-        <v>18.0</v>
+        <v>129.0</v>
       </c>
       <c r="L47" t="n">
-        <v>23.0</v>
+        <v>334.0</v>
       </c>
       <c r="M47" t="n">
-        <v>24.0</v>
+        <v>545.0</v>
       </c>
       <c r="N47" t="n">
-        <v>27.0</v>
+        <v>237.0</v>
       </c>
       <c r="O47" t="n">
-        <v>34.0</v>
+        <v>370.0</v>
       </c>
       <c r="P47" t="n">
-        <v>29.0</v>
+        <v>426.0</v>
       </c>
       <c r="Q47" t="n">
-        <v>65.0</v>
+        <v>534.0</v>
       </c>
     </row>
     <row r="48">
@@ -3723,49 +3723,49 @@
         <v>248</v>
       </c>
       <c r="C48" t="n">
-        <v>667.0</v>
+        <v>4932.0</v>
       </c>
       <c r="D48" t="n">
-        <v>664.0</v>
+        <v>4522.0</v>
       </c>
       <c r="E48" t="n">
-        <v>756.0</v>
+        <v>4659.0</v>
       </c>
       <c r="F48" t="n">
-        <v>398.0</v>
+        <v>1896.0</v>
       </c>
       <c r="G48" t="n">
-        <v>424.0</v>
+        <v>1895.0</v>
       </c>
       <c r="H48" t="n">
-        <v>334.0</v>
+        <v>2084.0</v>
       </c>
       <c r="I48" t="n">
-        <v>451.0</v>
+        <v>1500.0</v>
       </c>
       <c r="J48" t="n">
-        <v>362.0</v>
+        <v>720.0</v>
       </c>
       <c r="K48" t="n">
-        <v>129.0</v>
+        <v>1504.0</v>
       </c>
       <c r="L48" t="n">
-        <v>334.0</v>
+        <v>609.0</v>
       </c>
       <c r="M48" t="n">
-        <v>545.0</v>
+        <v>945.0</v>
       </c>
       <c r="N48" t="n">
-        <v>237.0</v>
+        <v>417.0</v>
       </c>
       <c r="O48" t="n">
-        <v>370.0</v>
+        <v>606.0</v>
       </c>
       <c r="P48" t="n">
-        <v>426.0</v>
+        <v>653.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>534.0</v>
+        <v>1156.0</v>
       </c>
     </row>
     <row r="49">
@@ -3776,49 +3776,49 @@
         <v>249</v>
       </c>
       <c r="C49" t="n">
-        <v>4932.0</v>
+        <v>2281.0</v>
       </c>
       <c r="D49" t="n">
-        <v>4522.0</v>
+        <v>1923.0</v>
       </c>
       <c r="E49" t="n">
-        <v>4659.0</v>
+        <v>1831.0</v>
       </c>
       <c r="F49" t="n">
-        <v>1896.0</v>
+        <v>1255.0</v>
       </c>
       <c r="G49" t="n">
-        <v>1895.0</v>
+        <v>1173.0</v>
       </c>
       <c r="H49" t="n">
-        <v>2084.0</v>
+        <v>1020.0</v>
       </c>
       <c r="I49" t="n">
-        <v>1500.0</v>
+        <v>1086.0</v>
       </c>
       <c r="J49" t="n">
-        <v>720.0</v>
+        <v>647.0</v>
       </c>
       <c r="K49" t="n">
-        <v>1504.0</v>
+        <v>569.0</v>
       </c>
       <c r="L49" t="n">
-        <v>609.0</v>
+        <v>614.0</v>
       </c>
       <c r="M49" t="n">
-        <v>945.0</v>
+        <v>672.0</v>
       </c>
       <c r="N49" t="n">
-        <v>417.0</v>
+        <v>164.0</v>
       </c>
       <c r="O49" t="n">
-        <v>606.0</v>
+        <v>688.0</v>
       </c>
       <c r="P49" t="n">
-        <v>653.0</v>
+        <v>667.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>1156.0</v>
+        <v>602.0</v>
       </c>
     </row>
     <row r="50">
@@ -3829,49 +3829,49 @@
         <v>250</v>
       </c>
       <c r="C50" t="n">
-        <v>2281.0</v>
+        <v>128.0</v>
       </c>
       <c r="D50" t="n">
-        <v>1923.0</v>
+        <v>165.0</v>
       </c>
       <c r="E50" t="n">
-        <v>1831.0</v>
+        <v>135.0</v>
       </c>
       <c r="F50" t="n">
-        <v>1255.0</v>
+        <v>67.0</v>
       </c>
       <c r="G50" t="n">
-        <v>1173.0</v>
+        <v>84.0</v>
       </c>
       <c r="H50" t="n">
-        <v>1020.0</v>
+        <v>31.0</v>
       </c>
       <c r="I50" t="n">
-        <v>1086.0</v>
+        <v>137.0</v>
       </c>
       <c r="J50" t="n">
-        <v>647.0</v>
+        <v>166.0</v>
       </c>
       <c r="K50" t="n">
-        <v>569.0</v>
+        <v>38.0</v>
       </c>
       <c r="L50" t="n">
-        <v>614.0</v>
+        <v>104.0</v>
       </c>
       <c r="M50" t="n">
-        <v>672.0</v>
+        <v>280.0</v>
       </c>
       <c r="N50" t="n">
-        <v>164.0</v>
+        <v>38.0</v>
       </c>
       <c r="O50" t="n">
-        <v>688.0</v>
+        <v>179.0</v>
       </c>
       <c r="P50" t="n">
-        <v>667.0</v>
+        <v>176.0</v>
       </c>
       <c r="Q50" t="n">
-        <v>602.0</v>
+        <v>235.0</v>
       </c>
     </row>
     <row r="51">
@@ -3882,49 +3882,49 @@
         <v>251</v>
       </c>
       <c r="C51" t="n">
-        <v>128.0</v>
+        <v>138.0</v>
       </c>
       <c r="D51" t="n">
-        <v>165.0</v>
+        <v>125.0</v>
       </c>
       <c r="E51" t="n">
-        <v>135.0</v>
+        <v>153.0</v>
       </c>
       <c r="F51" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>105.0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="J51" t="n">
         <v>67.0</v>
       </c>
-      <c r="G51" t="n">
-        <v>84.0</v>
-      </c>
-      <c r="H51" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="I51" t="n">
-        <v>137.0</v>
-      </c>
-      <c r="J51" t="n">
-        <v>166.0</v>
-      </c>
       <c r="K51" t="n">
-        <v>38.0</v>
+        <v>34.0</v>
       </c>
       <c r="L51" t="n">
-        <v>104.0</v>
+        <v>58.0</v>
       </c>
       <c r="M51" t="n">
-        <v>280.0</v>
+        <v>108.0</v>
       </c>
       <c r="N51" t="n">
-        <v>38.0</v>
+        <v>23.0</v>
       </c>
       <c r="O51" t="n">
-        <v>179.0</v>
+        <v>119.0</v>
       </c>
       <c r="P51" t="n">
-        <v>176.0</v>
+        <v>81.0</v>
       </c>
       <c r="Q51" t="n">
-        <v>235.0</v>
+        <v>116.0</v>
       </c>
     </row>
     <row r="52">
@@ -3935,49 +3935,49 @@
         <v>252</v>
       </c>
       <c r="C52" t="n">
-        <v>138.0</v>
+        <v>87.0</v>
       </c>
       <c r="D52" t="n">
-        <v>125.0</v>
+        <v>97.0</v>
       </c>
       <c r="E52" t="n">
-        <v>153.0</v>
+        <v>103.0</v>
       </c>
       <c r="F52" t="n">
-        <v>102.0</v>
+        <v>60.0</v>
       </c>
       <c r="G52" t="n">
-        <v>105.0</v>
+        <v>72.0</v>
       </c>
       <c r="H52" t="n">
-        <v>56.0</v>
+        <v>41.0</v>
       </c>
       <c r="I52" t="n">
-        <v>95.0</v>
+        <v>69.0</v>
       </c>
       <c r="J52" t="n">
-        <v>67.0</v>
+        <v>37.0</v>
       </c>
       <c r="K52" t="n">
-        <v>34.0</v>
+        <v>22.0</v>
       </c>
       <c r="L52" t="n">
-        <v>58.0</v>
+        <v>32.0</v>
       </c>
       <c r="M52" t="n">
-        <v>108.0</v>
+        <v>62.0</v>
       </c>
       <c r="N52" t="n">
-        <v>23.0</v>
+        <v>14.0</v>
       </c>
       <c r="O52" t="n">
-        <v>119.0</v>
+        <v>30.0</v>
       </c>
       <c r="P52" t="n">
-        <v>81.0</v>
+        <v>31.0</v>
       </c>
       <c r="Q52" t="n">
-        <v>116.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="53">
@@ -3988,49 +3988,49 @@
         <v>253</v>
       </c>
       <c r="C53" t="n">
-        <v>87.0</v>
+        <v>12.0</v>
       </c>
       <c r="D53" t="n">
-        <v>97.0</v>
+        <v>3.0</v>
       </c>
       <c r="E53" t="n">
-        <v>103.0</v>
+        <v>11.0</v>
       </c>
       <c r="F53" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="G53" t="n">
-        <v>72.0</v>
+        <v>2.0</v>
       </c>
       <c r="H53" t="n">
-        <v>41.0</v>
+        <v>1.0</v>
       </c>
       <c r="I53" t="n">
-        <v>69.0</v>
+        <v>0.0</v>
       </c>
       <c r="J53" t="n">
-        <v>37.0</v>
+        <v>0.0</v>
       </c>
       <c r="K53" t="n">
-        <v>22.0</v>
+        <v>0.0</v>
       </c>
       <c r="L53" t="n">
-        <v>32.0</v>
+        <v>2.0</v>
       </c>
       <c r="M53" t="n">
-        <v>62.0</v>
+        <v>1.0</v>
       </c>
       <c r="N53" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
       <c r="O53" t="n">
-        <v>30.0</v>
+        <v>0.0</v>
       </c>
       <c r="P53" t="n">
-        <v>31.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q53" t="n">
-        <v>39.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="54">
@@ -4041,49 +4041,49 @@
         <v>254</v>
       </c>
       <c r="C54" t="n">
+        <v>98.0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>79.0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="H54" t="n">
         <v>12.0</v>
       </c>
-      <c r="D54" t="n">
+      <c r="I54" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L54" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="M54" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="N54" t="n">
         <v>3.0</v>
       </c>
-      <c r="E54" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G54" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H54" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L54" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="M54" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="N54" t="n">
-        <v>0.0</v>
-      </c>
       <c r="O54" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="P54" t="n">
         <v>0.0</v>
       </c>
       <c r="Q54" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="55">
@@ -4094,49 +4094,49 @@
         <v>255</v>
       </c>
       <c r="C55" t="n">
-        <v>98.0</v>
+        <v>84.0</v>
       </c>
       <c r="D55" t="n">
-        <v>79.0</v>
+        <v>89.0</v>
       </c>
       <c r="E55" t="n">
-        <v>38.0</v>
+        <v>70.0</v>
       </c>
       <c r="F55" t="n">
-        <v>28.0</v>
+        <v>42.0</v>
       </c>
       <c r="G55" t="n">
-        <v>49.0</v>
+        <v>80.0</v>
       </c>
       <c r="H55" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="K55" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="L55" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="M55" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="N55" t="n">
         <v>12.0</v>
       </c>
-      <c r="I55" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="J55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K55" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="L55" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="M55" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="N55" t="n">
-        <v>3.0</v>
-      </c>
       <c r="O55" t="n">
-        <v>2.0</v>
+        <v>78.0</v>
       </c>
       <c r="P55" t="n">
-        <v>0.0</v>
+        <v>31.0</v>
       </c>
       <c r="Q55" t="n">
-        <v>4.0</v>
+        <v>137.0</v>
       </c>
     </row>
     <row r="56">
@@ -4147,49 +4147,49 @@
         <v>256</v>
       </c>
       <c r="C56" t="n">
-        <v>84.0</v>
+        <v>1290.0</v>
       </c>
       <c r="D56" t="n">
-        <v>89.0</v>
+        <v>1510.0</v>
       </c>
       <c r="E56" t="n">
-        <v>70.0</v>
+        <v>1798.0</v>
       </c>
       <c r="F56" t="n">
-        <v>42.0</v>
+        <v>902.0</v>
       </c>
       <c r="G56" t="n">
-        <v>80.0</v>
+        <v>1123.0</v>
       </c>
       <c r="H56" t="n">
-        <v>33.0</v>
+        <v>374.0</v>
       </c>
       <c r="I56" t="n">
-        <v>64.0</v>
+        <v>1029.0</v>
       </c>
       <c r="J56" t="n">
-        <v>41.0</v>
+        <v>745.0</v>
       </c>
       <c r="K56" t="n">
-        <v>31.0</v>
+        <v>248.0</v>
       </c>
       <c r="L56" t="n">
-        <v>44.0</v>
+        <v>684.0</v>
       </c>
       <c r="M56" t="n">
-        <v>52.0</v>
+        <v>839.0</v>
       </c>
       <c r="N56" t="n">
-        <v>12.0</v>
+        <v>359.0</v>
       </c>
       <c r="O56" t="n">
-        <v>78.0</v>
+        <v>782.0</v>
       </c>
       <c r="P56" t="n">
-        <v>31.0</v>
+        <v>591.0</v>
       </c>
       <c r="Q56" t="n">
-        <v>137.0</v>
+        <v>876.0</v>
       </c>
     </row>
     <row r="57">
@@ -4200,49 +4200,49 @@
         <v>257</v>
       </c>
       <c r="C57" t="n">
-        <v>1290.0</v>
+        <v>2887.0</v>
       </c>
       <c r="D57" t="n">
-        <v>1510.0</v>
+        <v>2933.0</v>
       </c>
       <c r="E57" t="n">
-        <v>1798.0</v>
+        <v>3213.0</v>
       </c>
       <c r="F57" t="n">
-        <v>902.0</v>
+        <v>2084.0</v>
       </c>
       <c r="G57" t="n">
-        <v>1123.0</v>
+        <v>2392.0</v>
       </c>
       <c r="H57" t="n">
-        <v>374.0</v>
+        <v>1289.0</v>
       </c>
       <c r="I57" t="n">
-        <v>1029.0</v>
+        <v>2409.0</v>
       </c>
       <c r="J57" t="n">
-        <v>745.0</v>
+        <v>1733.0</v>
       </c>
       <c r="K57" t="n">
-        <v>248.0</v>
+        <v>910.0</v>
       </c>
       <c r="L57" t="n">
-        <v>684.0</v>
+        <v>1476.0</v>
       </c>
       <c r="M57" t="n">
-        <v>839.0</v>
+        <v>2470.0</v>
       </c>
       <c r="N57" t="n">
-        <v>359.0</v>
+        <v>1141.0</v>
       </c>
       <c r="O57" t="n">
-        <v>782.0</v>
+        <v>1670.0</v>
       </c>
       <c r="P57" t="n">
-        <v>591.0</v>
+        <v>1931.0</v>
       </c>
       <c r="Q57" t="n">
-        <v>876.0</v>
+        <v>3575.0</v>
       </c>
     </row>
     <row r="58">
@@ -4253,49 +4253,49 @@
         <v>258</v>
       </c>
       <c r="C58" t="n">
-        <v>2887.0</v>
+        <v>30.0</v>
       </c>
       <c r="D58" t="n">
-        <v>2933.0</v>
+        <v>40.0</v>
       </c>
       <c r="E58" t="n">
-        <v>3213.0</v>
+        <v>20.0</v>
       </c>
       <c r="F58" t="n">
-        <v>2084.0</v>
+        <v>4.0</v>
       </c>
       <c r="G58" t="n">
-        <v>2392.0</v>
+        <v>6.0</v>
       </c>
       <c r="H58" t="n">
-        <v>1289.0</v>
+        <v>4.0</v>
       </c>
       <c r="I58" t="n">
-        <v>2409.0</v>
+        <v>4.0</v>
       </c>
       <c r="J58" t="n">
-        <v>1733.0</v>
+        <v>2.0</v>
       </c>
       <c r="K58" t="n">
-        <v>910.0</v>
+        <v>6.0</v>
       </c>
       <c r="L58" t="n">
-        <v>1476.0</v>
+        <v>0.0</v>
       </c>
       <c r="M58" t="n">
-        <v>2470.0</v>
+        <v>0.0</v>
       </c>
       <c r="N58" t="n">
-        <v>1141.0</v>
+        <v>2.0</v>
       </c>
       <c r="O58" t="n">
-        <v>1670.0</v>
+        <v>0.0</v>
       </c>
       <c r="P58" t="n">
-        <v>1931.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q58" t="n">
-        <v>3575.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="59">
@@ -4306,49 +4306,49 @@
         <v>259</v>
       </c>
       <c r="C59" t="n">
-        <v>30.0</v>
+        <v>593.0</v>
       </c>
       <c r="D59" t="n">
-        <v>40.0</v>
+        <v>568.0</v>
       </c>
       <c r="E59" t="n">
-        <v>20.0</v>
+        <v>539.0</v>
       </c>
       <c r="F59" t="n">
-        <v>4.0</v>
+        <v>482.0</v>
       </c>
       <c r="G59" t="n">
-        <v>6.0</v>
+        <v>528.0</v>
       </c>
       <c r="H59" t="n">
-        <v>4.0</v>
+        <v>161.0</v>
       </c>
       <c r="I59" t="n">
-        <v>4.0</v>
+        <v>454.0</v>
       </c>
       <c r="J59" t="n">
-        <v>2.0</v>
+        <v>399.0</v>
       </c>
       <c r="K59" t="n">
-        <v>6.0</v>
+        <v>117.0</v>
       </c>
       <c r="L59" t="n">
-        <v>0.0</v>
+        <v>365.0</v>
       </c>
       <c r="M59" t="n">
-        <v>0.0</v>
+        <v>396.0</v>
       </c>
       <c r="N59" t="n">
-        <v>2.0</v>
+        <v>333.0</v>
       </c>
       <c r="O59" t="n">
-        <v>0.0</v>
+        <v>423.0</v>
       </c>
       <c r="P59" t="n">
-        <v>0.0</v>
+        <v>383.0</v>
       </c>
       <c r="Q59" t="n">
-        <v>0.0</v>
+        <v>669.0</v>
       </c>
     </row>
     <row r="60">
@@ -4359,49 +4359,49 @@
         <v>260</v>
       </c>
       <c r="C60" t="n">
-        <v>593.0</v>
+        <v>36.0</v>
       </c>
       <c r="D60" t="n">
-        <v>568.0</v>
+        <v>42.0</v>
       </c>
       <c r="E60" t="n">
-        <v>539.0</v>
+        <v>74.0</v>
       </c>
       <c r="F60" t="n">
-        <v>482.0</v>
+        <v>27.0</v>
       </c>
       <c r="G60" t="n">
-        <v>528.0</v>
+        <v>38.0</v>
       </c>
       <c r="H60" t="n">
-        <v>161.0</v>
+        <v>10.0</v>
       </c>
       <c r="I60" t="n">
-        <v>454.0</v>
+        <v>32.0</v>
       </c>
       <c r="J60" t="n">
-        <v>399.0</v>
+        <v>20.0</v>
       </c>
       <c r="K60" t="n">
-        <v>117.0</v>
+        <v>19.0</v>
       </c>
       <c r="L60" t="n">
-        <v>365.0</v>
+        <v>20.0</v>
       </c>
       <c r="M60" t="n">
-        <v>396.0</v>
+        <v>30.0</v>
       </c>
       <c r="N60" t="n">
-        <v>333.0</v>
+        <v>16.0</v>
       </c>
       <c r="O60" t="n">
-        <v>423.0</v>
+        <v>39.0</v>
       </c>
       <c r="P60" t="n">
-        <v>383.0</v>
+        <v>6.0</v>
       </c>
       <c r="Q60" t="n">
-        <v>669.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="61">
@@ -4412,49 +4412,49 @@
         <v>261</v>
       </c>
       <c r="C61" t="n">
-        <v>36.0</v>
+        <v>29.0</v>
       </c>
       <c r="D61" t="n">
-        <v>42.0</v>
+        <v>19.0</v>
       </c>
       <c r="E61" t="n">
-        <v>74.0</v>
+        <v>20.0</v>
       </c>
       <c r="F61" t="n">
-        <v>27.0</v>
+        <v>8.0</v>
       </c>
       <c r="G61" t="n">
-        <v>38.0</v>
+        <v>15.0</v>
       </c>
       <c r="H61" t="n">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c r="I61" t="n">
-        <v>32.0</v>
+        <v>19.0</v>
       </c>
       <c r="J61" t="n">
-        <v>20.0</v>
+        <v>4.0</v>
       </c>
       <c r="K61" t="n">
-        <v>19.0</v>
+        <v>4.0</v>
       </c>
       <c r="L61" t="n">
-        <v>20.0</v>
+        <v>4.0</v>
       </c>
       <c r="M61" t="n">
-        <v>30.0</v>
+        <v>0.0</v>
       </c>
       <c r="N61" t="n">
-        <v>16.0</v>
+        <v>2.0</v>
       </c>
       <c r="O61" t="n">
-        <v>39.0</v>
+        <v>2.0</v>
       </c>
       <c r="P61" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q61" t="n">
-        <v>48.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="62">
@@ -4465,49 +4465,49 @@
         <v>262</v>
       </c>
       <c r="C62" t="n">
-        <v>29.0</v>
+        <v>10.0</v>
       </c>
       <c r="D62" t="n">
-        <v>19.0</v>
+        <v>14.0</v>
       </c>
       <c r="E62" t="n">
-        <v>20.0</v>
+        <v>23.0</v>
       </c>
       <c r="F62" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H62" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K62" t="n">
         <v>8.0</v>
       </c>
-      <c r="G62" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="H62" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I62" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="J62" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="K62" t="n">
-        <v>4.0</v>
-      </c>
       <c r="L62" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="M62" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="N62" t="n">
         <v>2.0</v>
       </c>
       <c r="O62" t="n">
-        <v>2.0</v>
+        <v>11.0</v>
       </c>
       <c r="P62" t="n">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
       <c r="Q62" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="63">
@@ -4518,49 +4518,49 @@
         <v>263</v>
       </c>
       <c r="C63" t="n">
-        <v>10.0</v>
+        <v>548.0</v>
       </c>
       <c r="D63" t="n">
-        <v>14.0</v>
+        <v>506.0</v>
       </c>
       <c r="E63" t="n">
-        <v>23.0</v>
+        <v>510.0</v>
       </c>
       <c r="F63" t="n">
-        <v>9.0</v>
+        <v>370.0</v>
       </c>
       <c r="G63" t="n">
-        <v>6.0</v>
+        <v>323.0</v>
       </c>
       <c r="H63" t="n">
-        <v>4.0</v>
+        <v>198.0</v>
       </c>
       <c r="I63" t="n">
-        <v>9.0</v>
+        <v>304.0</v>
       </c>
       <c r="J63" t="n">
-        <v>5.0</v>
+        <v>101.0</v>
       </c>
       <c r="K63" t="n">
-        <v>8.0</v>
+        <v>84.0</v>
       </c>
       <c r="L63" t="n">
-        <v>8.0</v>
+        <v>104.0</v>
       </c>
       <c r="M63" t="n">
-        <v>5.0</v>
+        <v>78.0</v>
       </c>
       <c r="N63" t="n">
-        <v>2.0</v>
+        <v>38.0</v>
       </c>
       <c r="O63" t="n">
-        <v>11.0</v>
+        <v>86.0</v>
       </c>
       <c r="P63" t="n">
-        <v>11.0</v>
+        <v>71.0</v>
       </c>
       <c r="Q63" t="n">
-        <v>10.0</v>
+        <v>160.0</v>
       </c>
     </row>
     <row r="64">
@@ -4571,49 +4571,49 @@
         <v>264</v>
       </c>
       <c r="C64" t="n">
-        <v>548.0</v>
+        <v>37.0</v>
       </c>
       <c r="D64" t="n">
-        <v>506.0</v>
+        <v>25.0</v>
       </c>
       <c r="E64" t="n">
-        <v>510.0</v>
+        <v>33.0</v>
       </c>
       <c r="F64" t="n">
-        <v>370.0</v>
+        <v>10.0</v>
       </c>
       <c r="G64" t="n">
-        <v>323.0</v>
+        <v>4.0</v>
       </c>
       <c r="H64" t="n">
-        <v>198.0</v>
+        <v>9.0</v>
       </c>
       <c r="I64" t="n">
-        <v>304.0</v>
+        <v>14.0</v>
       </c>
       <c r="J64" t="n">
-        <v>101.0</v>
+        <v>10.0</v>
       </c>
       <c r="K64" t="n">
-        <v>84.0</v>
+        <v>13.0</v>
       </c>
       <c r="L64" t="n">
-        <v>104.0</v>
+        <v>7.0</v>
       </c>
       <c r="M64" t="n">
-        <v>78.0</v>
+        <v>16.0</v>
       </c>
       <c r="N64" t="n">
-        <v>38.0</v>
+        <v>14.0</v>
       </c>
       <c r="O64" t="n">
-        <v>86.0</v>
+        <v>10.0</v>
       </c>
       <c r="P64" t="n">
-        <v>71.0</v>
+        <v>6.0</v>
       </c>
       <c r="Q64" t="n">
-        <v>160.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="65">
@@ -4624,49 +4624,49 @@
         <v>265</v>
       </c>
       <c r="C65" t="n">
-        <v>37.0</v>
+        <v>2157.0</v>
       </c>
       <c r="D65" t="n">
-        <v>25.0</v>
+        <v>2108.0</v>
       </c>
       <c r="E65" t="n">
-        <v>33.0</v>
+        <v>1833.0</v>
       </c>
       <c r="F65" t="n">
-        <v>10.0</v>
+        <v>1580.0</v>
       </c>
       <c r="G65" t="n">
-        <v>4.0</v>
+        <v>1558.0</v>
       </c>
       <c r="H65" t="n">
-        <v>9.0</v>
+        <v>703.0</v>
       </c>
       <c r="I65" t="n">
-        <v>14.0</v>
+        <v>1322.0</v>
       </c>
       <c r="J65" t="n">
-        <v>10.0</v>
+        <v>791.0</v>
       </c>
       <c r="K65" t="n">
-        <v>13.0</v>
+        <v>381.0</v>
       </c>
       <c r="L65" t="n">
-        <v>7.0</v>
+        <v>605.0</v>
       </c>
       <c r="M65" t="n">
-        <v>16.0</v>
+        <v>933.0</v>
       </c>
       <c r="N65" t="n">
-        <v>14.0</v>
+        <v>362.0</v>
       </c>
       <c r="O65" t="n">
-        <v>10.0</v>
+        <v>706.0</v>
       </c>
       <c r="P65" t="n">
-        <v>6.0</v>
+        <v>519.0</v>
       </c>
       <c r="Q65" t="n">
-        <v>31.0</v>
+        <v>1307.0</v>
       </c>
     </row>
     <row r="66">
@@ -4677,49 +4677,49 @@
         <v>266</v>
       </c>
       <c r="C66" t="n">
-        <v>2157.0</v>
+        <v>543.0</v>
       </c>
       <c r="D66" t="n">
-        <v>2108.0</v>
+        <v>641.0</v>
       </c>
       <c r="E66" t="n">
-        <v>1833.0</v>
+        <v>750.0</v>
       </c>
       <c r="F66" t="n">
-        <v>1580.0</v>
+        <v>478.0</v>
       </c>
       <c r="G66" t="n">
-        <v>1558.0</v>
+        <v>511.0</v>
       </c>
       <c r="H66" t="n">
-        <v>703.0</v>
+        <v>256.0</v>
       </c>
       <c r="I66" t="n">
-        <v>1322.0</v>
+        <v>526.0</v>
       </c>
       <c r="J66" t="n">
-        <v>791.0</v>
+        <v>415.0</v>
       </c>
       <c r="K66" t="n">
-        <v>381.0</v>
+        <v>174.0</v>
       </c>
       <c r="L66" t="n">
-        <v>605.0</v>
+        <v>314.0</v>
       </c>
       <c r="M66" t="n">
-        <v>933.0</v>
+        <v>693.0</v>
       </c>
       <c r="N66" t="n">
-        <v>362.0</v>
+        <v>425.0</v>
       </c>
       <c r="O66" t="n">
-        <v>706.0</v>
+        <v>404.0</v>
       </c>
       <c r="P66" t="n">
-        <v>519.0</v>
+        <v>443.0</v>
       </c>
       <c r="Q66" t="n">
-        <v>1307.0</v>
+        <v>798.0</v>
       </c>
     </row>
     <row r="67">
@@ -4730,49 +4730,49 @@
         <v>267</v>
       </c>
       <c r="C67" t="n">
-        <v>543.0</v>
+        <v>162.0</v>
       </c>
       <c r="D67" t="n">
-        <v>641.0</v>
+        <v>284.0</v>
       </c>
       <c r="E67" t="n">
-        <v>750.0</v>
+        <v>54.0</v>
       </c>
       <c r="F67" t="n">
-        <v>478.0</v>
+        <v>54.0</v>
       </c>
       <c r="G67" t="n">
-        <v>511.0</v>
+        <v>53.0</v>
       </c>
       <c r="H67" t="n">
-        <v>256.0</v>
+        <v>22.0</v>
       </c>
       <c r="I67" t="n">
-        <v>526.0</v>
+        <v>37.0</v>
       </c>
       <c r="J67" t="n">
-        <v>415.0</v>
+        <v>5.0</v>
       </c>
       <c r="K67" t="n">
-        <v>174.0</v>
+        <v>8.0</v>
       </c>
       <c r="L67" t="n">
-        <v>314.0</v>
+        <v>2.0</v>
       </c>
       <c r="M67" t="n">
-        <v>693.0</v>
+        <v>0.0</v>
       </c>
       <c r="N67" t="n">
-        <v>425.0</v>
+        <v>0.0</v>
       </c>
       <c r="O67" t="n">
-        <v>404.0</v>
+        <v>0.0</v>
       </c>
       <c r="P67" t="n">
-        <v>443.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q67" t="n">
-        <v>798.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="68">
@@ -4783,49 +4783,49 @@
         <v>268</v>
       </c>
       <c r="C68" t="n">
-        <v>162.0</v>
+        <v>86.0</v>
       </c>
       <c r="D68" t="n">
-        <v>284.0</v>
+        <v>91.0</v>
       </c>
       <c r="E68" t="n">
-        <v>54.0</v>
+        <v>107.0</v>
       </c>
       <c r="F68" t="n">
-        <v>54.0</v>
+        <v>32.0</v>
       </c>
       <c r="G68" t="n">
-        <v>53.0</v>
+        <v>62.0</v>
       </c>
       <c r="H68" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="J68" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="K68" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="L68" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="M68" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="N68" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="O68" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="P68" t="n">
         <v>22.0</v>
       </c>
-      <c r="I68" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="J68" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="K68" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="L68" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="M68" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N68" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O68" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P68" t="n">
-        <v>0.0</v>
-      </c>
       <c r="Q68" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="69">
@@ -4836,49 +4836,49 @@
         <v>269</v>
       </c>
       <c r="C69" t="n">
-        <v>86.0</v>
+        <v>267.0</v>
       </c>
       <c r="D69" t="n">
-        <v>91.0</v>
+        <v>346.0</v>
       </c>
       <c r="E69" t="n">
-        <v>107.0</v>
+        <v>384.0</v>
       </c>
       <c r="F69" t="n">
-        <v>32.0</v>
+        <v>88.0</v>
       </c>
       <c r="G69" t="n">
-        <v>62.0</v>
+        <v>156.0</v>
       </c>
       <c r="H69" t="n">
-        <v>28.0</v>
+        <v>155.0</v>
       </c>
       <c r="I69" t="n">
-        <v>50.0</v>
+        <v>169.0</v>
       </c>
       <c r="J69" t="n">
-        <v>25.0</v>
+        <v>129.0</v>
       </c>
       <c r="K69" t="n">
-        <v>36.0</v>
+        <v>99.0</v>
       </c>
       <c r="L69" t="n">
-        <v>44.0</v>
+        <v>69.0</v>
       </c>
       <c r="M69" t="n">
-        <v>33.0</v>
+        <v>148.0</v>
       </c>
       <c r="N69" t="n">
-        <v>47.0</v>
+        <v>51.0</v>
       </c>
       <c r="O69" t="n">
-        <v>30.0</v>
+        <v>92.0</v>
       </c>
       <c r="P69" t="n">
-        <v>22.0</v>
+        <v>103.0</v>
       </c>
       <c r="Q69" t="n">
-        <v>50.0</v>
+        <v>387.0</v>
       </c>
     </row>
     <row r="70">
@@ -4889,49 +4889,49 @@
         <v>270</v>
       </c>
       <c r="C70" t="n">
-        <v>267.0</v>
+        <v>190.0</v>
       </c>
       <c r="D70" t="n">
-        <v>346.0</v>
+        <v>313.0</v>
       </c>
       <c r="E70" t="n">
-        <v>384.0</v>
+        <v>130.0</v>
       </c>
       <c r="F70" t="n">
-        <v>88.0</v>
+        <v>72.0</v>
       </c>
       <c r="G70" t="n">
-        <v>156.0</v>
+        <v>78.0</v>
       </c>
       <c r="H70" t="n">
-        <v>155.0</v>
+        <v>10.0</v>
       </c>
       <c r="I70" t="n">
-        <v>169.0</v>
+        <v>60.0</v>
       </c>
       <c r="J70" t="n">
-        <v>129.0</v>
+        <v>4.0</v>
       </c>
       <c r="K70" t="n">
-        <v>99.0</v>
+        <v>4.0</v>
       </c>
       <c r="L70" t="n">
-        <v>69.0</v>
+        <v>3.0</v>
       </c>
       <c r="M70" t="n">
-        <v>148.0</v>
+        <v>0.0</v>
       </c>
       <c r="N70" t="n">
-        <v>51.0</v>
+        <v>8.0</v>
       </c>
       <c r="O70" t="n">
-        <v>92.0</v>
+        <v>6.0</v>
       </c>
       <c r="P70" t="n">
-        <v>103.0</v>
+        <v>2.0</v>
       </c>
       <c r="Q70" t="n">
-        <v>387.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="71">
@@ -4942,49 +4942,49 @@
         <v>271</v>
       </c>
       <c r="C71" t="n">
-        <v>190.0</v>
+        <v>424.0</v>
       </c>
       <c r="D71" t="n">
-        <v>313.0</v>
+        <v>401.0</v>
       </c>
       <c r="E71" t="n">
-        <v>130.0</v>
+        <v>466.0</v>
       </c>
       <c r="F71" t="n">
-        <v>72.0</v>
+        <v>362.0</v>
       </c>
       <c r="G71" t="n">
-        <v>78.0</v>
+        <v>404.0</v>
       </c>
       <c r="H71" t="n">
-        <v>10.0</v>
+        <v>117.0</v>
       </c>
       <c r="I71" t="n">
-        <v>60.0</v>
+        <v>316.0</v>
       </c>
       <c r="J71" t="n">
-        <v>4.0</v>
+        <v>122.0</v>
       </c>
       <c r="K71" t="n">
-        <v>4.0</v>
+        <v>65.0</v>
       </c>
       <c r="L71" t="n">
-        <v>3.0</v>
+        <v>92.0</v>
       </c>
       <c r="M71" t="n">
-        <v>0.0</v>
+        <v>86.0</v>
       </c>
       <c r="N71" t="n">
-        <v>8.0</v>
+        <v>24.0</v>
       </c>
       <c r="O71" t="n">
-        <v>6.0</v>
+        <v>122.0</v>
       </c>
       <c r="P71" t="n">
-        <v>2.0</v>
+        <v>62.0</v>
       </c>
       <c r="Q71" t="n">
-        <v>1.0</v>
+        <v>127.0</v>
       </c>
     </row>
     <row r="72">
@@ -4995,49 +4995,49 @@
         <v>272</v>
       </c>
       <c r="C72" t="n">
-        <v>424.0</v>
+        <v>190.0</v>
       </c>
       <c r="D72" t="n">
-        <v>401.0</v>
+        <v>206.0</v>
       </c>
       <c r="E72" t="n">
-        <v>466.0</v>
+        <v>109.0</v>
       </c>
       <c r="F72" t="n">
-        <v>362.0</v>
+        <v>58.0</v>
       </c>
       <c r="G72" t="n">
-        <v>404.0</v>
+        <v>66.0</v>
       </c>
       <c r="H72" t="n">
-        <v>117.0</v>
+        <v>8.0</v>
       </c>
       <c r="I72" t="n">
-        <v>316.0</v>
+        <v>26.0</v>
       </c>
       <c r="J72" t="n">
-        <v>122.0</v>
+        <v>6.0</v>
       </c>
       <c r="K72" t="n">
-        <v>65.0</v>
+        <v>12.0</v>
       </c>
       <c r="L72" t="n">
-        <v>92.0</v>
+        <v>13.0</v>
       </c>
       <c r="M72" t="n">
-        <v>86.0</v>
+        <v>10.0</v>
       </c>
       <c r="N72" t="n">
-        <v>24.0</v>
+        <v>18.0</v>
       </c>
       <c r="O72" t="n">
-        <v>122.0</v>
+        <v>5.0</v>
       </c>
       <c r="P72" t="n">
-        <v>62.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q72" t="n">
-        <v>127.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="73">
@@ -5048,49 +5048,49 @@
         <v>273</v>
       </c>
       <c r="C73" t="n">
-        <v>190.0</v>
+        <v>179.0</v>
       </c>
       <c r="D73" t="n">
-        <v>206.0</v>
+        <v>128.0</v>
       </c>
       <c r="E73" t="n">
-        <v>109.0</v>
+        <v>165.0</v>
       </c>
       <c r="F73" t="n">
-        <v>58.0</v>
+        <v>94.0</v>
       </c>
       <c r="G73" t="n">
-        <v>66.0</v>
+        <v>70.0</v>
       </c>
       <c r="H73" t="n">
-        <v>8.0</v>
+        <v>50.0</v>
       </c>
       <c r="I73" t="n">
-        <v>26.0</v>
+        <v>63.0</v>
       </c>
       <c r="J73" t="n">
-        <v>6.0</v>
+        <v>31.0</v>
       </c>
       <c r="K73" t="n">
-        <v>12.0</v>
+        <v>32.0</v>
       </c>
       <c r="L73" t="n">
-        <v>13.0</v>
+        <v>18.0</v>
       </c>
       <c r="M73" t="n">
-        <v>10.0</v>
+        <v>24.0</v>
       </c>
       <c r="N73" t="n">
-        <v>18.0</v>
+        <v>17.0</v>
       </c>
       <c r="O73" t="n">
-        <v>5.0</v>
+        <v>32.0</v>
       </c>
       <c r="P73" t="n">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
       <c r="Q73" t="n">
-        <v>6.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="74">
@@ -5101,49 +5101,49 @@
         <v>274</v>
       </c>
       <c r="C74" t="n">
-        <v>179.0</v>
+        <v>17.0</v>
       </c>
       <c r="D74" t="n">
-        <v>128.0</v>
+        <v>19.0</v>
       </c>
       <c r="E74" t="n">
-        <v>165.0</v>
+        <v>15.0</v>
       </c>
       <c r="F74" t="n">
-        <v>94.0</v>
+        <v>8.0</v>
       </c>
       <c r="G74" t="n">
-        <v>70.0</v>
+        <v>5.0</v>
       </c>
       <c r="H74" t="n">
-        <v>50.0</v>
+        <v>2.0</v>
       </c>
       <c r="I74" t="n">
-        <v>63.0</v>
+        <v>5.0</v>
       </c>
       <c r="J74" t="n">
-        <v>31.0</v>
+        <v>9.0</v>
       </c>
       <c r="K74" t="n">
-        <v>32.0</v>
+        <v>8.0</v>
       </c>
       <c r="L74" t="n">
-        <v>18.0</v>
+        <v>2.0</v>
       </c>
       <c r="M74" t="n">
-        <v>24.0</v>
+        <v>5.0</v>
       </c>
       <c r="N74" t="n">
-        <v>17.0</v>
+        <v>1.0</v>
       </c>
       <c r="O74" t="n">
-        <v>32.0</v>
+        <v>5.0</v>
       </c>
       <c r="P74" t="n">
-        <v>14.0</v>
+        <v>8.0</v>
       </c>
       <c r="Q74" t="n">
-        <v>52.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="75">
@@ -5154,49 +5154,49 @@
         <v>275</v>
       </c>
       <c r="C75" t="n">
-        <v>17.0</v>
+        <v>156.0</v>
       </c>
       <c r="D75" t="n">
-        <v>19.0</v>
+        <v>119.0</v>
       </c>
       <c r="E75" t="n">
-        <v>15.0</v>
+        <v>212.0</v>
       </c>
       <c r="F75" t="n">
-        <v>8.0</v>
+        <v>92.0</v>
       </c>
       <c r="G75" t="n">
-        <v>5.0</v>
+        <v>103.0</v>
       </c>
       <c r="H75" t="n">
-        <v>2.0</v>
+        <v>85.0</v>
       </c>
       <c r="I75" t="n">
-        <v>5.0</v>
+        <v>146.0</v>
       </c>
       <c r="J75" t="n">
-        <v>9.0</v>
+        <v>131.0</v>
       </c>
       <c r="K75" t="n">
-        <v>8.0</v>
+        <v>71.0</v>
       </c>
       <c r="L75" t="n">
-        <v>2.0</v>
+        <v>108.0</v>
       </c>
       <c r="M75" t="n">
-        <v>5.0</v>
+        <v>141.0</v>
       </c>
       <c r="N75" t="n">
-        <v>1.0</v>
+        <v>44.0</v>
       </c>
       <c r="O75" t="n">
-        <v>5.0</v>
+        <v>153.0</v>
       </c>
       <c r="P75" t="n">
-        <v>8.0</v>
+        <v>114.0</v>
       </c>
       <c r="Q75" t="n">
-        <v>0.0</v>
+        <v>76.0</v>
       </c>
     </row>
     <row r="76">
@@ -5207,49 +5207,49 @@
         <v>276</v>
       </c>
       <c r="C76" t="n">
-        <v>156.0</v>
+        <v>102.0</v>
       </c>
       <c r="D76" t="n">
-        <v>119.0</v>
+        <v>117.0</v>
       </c>
       <c r="E76" t="n">
-        <v>212.0</v>
+        <v>67.0</v>
       </c>
       <c r="F76" t="n">
-        <v>92.0</v>
+        <v>35.0</v>
       </c>
       <c r="G76" t="n">
-        <v>103.0</v>
+        <v>65.0</v>
       </c>
       <c r="H76" t="n">
-        <v>85.0</v>
+        <v>30.0</v>
       </c>
       <c r="I76" t="n">
-        <v>146.0</v>
+        <v>55.0</v>
       </c>
       <c r="J76" t="n">
-        <v>131.0</v>
+        <v>61.0</v>
       </c>
       <c r="K76" t="n">
-        <v>71.0</v>
+        <v>24.0</v>
       </c>
       <c r="L76" t="n">
-        <v>108.0</v>
+        <v>64.0</v>
       </c>
       <c r="M76" t="n">
-        <v>141.0</v>
+        <v>43.0</v>
       </c>
       <c r="N76" t="n">
-        <v>44.0</v>
+        <v>34.0</v>
       </c>
       <c r="O76" t="n">
-        <v>153.0</v>
+        <v>65.0</v>
       </c>
       <c r="P76" t="n">
-        <v>114.0</v>
+        <v>48.0</v>
       </c>
       <c r="Q76" t="n">
-        <v>76.0</v>
+        <v>159.0</v>
       </c>
     </row>
     <row r="77">
@@ -5260,49 +5260,49 @@
         <v>277</v>
       </c>
       <c r="C77" t="n">
-        <v>102.0</v>
+        <v>435.0</v>
       </c>
       <c r="D77" t="n">
+        <v>424.0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>487.0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>350.0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>326.0</v>
+      </c>
+      <c r="H77" t="n">
+        <v>136.0</v>
+      </c>
+      <c r="I77" t="n">
+        <v>307.0</v>
+      </c>
+      <c r="J77" t="n">
+        <v>155.0</v>
+      </c>
+      <c r="K77" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="L77" t="n">
+        <v>146.0</v>
+      </c>
+      <c r="M77" t="n">
+        <v>94.0</v>
+      </c>
+      <c r="N77" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="O77" t="n">
         <v>117.0</v>
       </c>
-      <c r="E77" t="n">
-        <v>67.0</v>
-      </c>
-      <c r="F77" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="G77" t="n">
-        <v>65.0</v>
-      </c>
-      <c r="H77" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="I77" t="n">
-        <v>55.0</v>
-      </c>
-      <c r="J77" t="n">
-        <v>61.0</v>
-      </c>
-      <c r="K77" t="n">
-        <v>24.0</v>
-      </c>
-      <c r="L77" t="n">
-        <v>64.0</v>
-      </c>
-      <c r="M77" t="n">
-        <v>43.0</v>
-      </c>
-      <c r="N77" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="O77" t="n">
-        <v>65.0</v>
-      </c>
       <c r="P77" t="n">
-        <v>48.0</v>
+        <v>145.0</v>
       </c>
       <c r="Q77" t="n">
-        <v>159.0</v>
+        <v>214.0</v>
       </c>
     </row>
     <row r="78">
@@ -5313,49 +5313,49 @@
         <v>278</v>
       </c>
       <c r="C78" t="n">
-        <v>435.0</v>
+        <v>36.0</v>
       </c>
       <c r="D78" t="n">
-        <v>424.0</v>
+        <v>35.0</v>
       </c>
       <c r="E78" t="n">
-        <v>487.0</v>
+        <v>31.0</v>
       </c>
       <c r="F78" t="n">
-        <v>350.0</v>
+        <v>15.0</v>
       </c>
       <c r="G78" t="n">
-        <v>326.0</v>
+        <v>18.0</v>
       </c>
       <c r="H78" t="n">
-        <v>136.0</v>
+        <v>10.0</v>
       </c>
       <c r="I78" t="n">
-        <v>307.0</v>
+        <v>20.0</v>
       </c>
       <c r="J78" t="n">
-        <v>155.0</v>
+        <v>9.0</v>
       </c>
       <c r="K78" t="n">
-        <v>80.0</v>
+        <v>2.0</v>
       </c>
       <c r="L78" t="n">
-        <v>146.0</v>
+        <v>18.0</v>
       </c>
       <c r="M78" t="n">
-        <v>94.0</v>
+        <v>20.0</v>
       </c>
       <c r="N78" t="n">
-        <v>49.0</v>
+        <v>4.0</v>
       </c>
       <c r="O78" t="n">
-        <v>117.0</v>
+        <v>17.0</v>
       </c>
       <c r="P78" t="n">
-        <v>145.0</v>
+        <v>9.0</v>
       </c>
       <c r="Q78" t="n">
-        <v>214.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="79">
@@ -5366,49 +5366,49 @@
         <v>279</v>
       </c>
       <c r="C79" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="D79" t="n">
         <v>36.0</v>
-      </c>
-      <c r="D79" t="n">
-        <v>35.0</v>
       </c>
       <c r="E79" t="n">
         <v>31.0</v>
       </c>
       <c r="F79" t="n">
-        <v>15.0</v>
+        <v>21.0</v>
       </c>
       <c r="G79" t="n">
-        <v>18.0</v>
+        <v>43.0</v>
       </c>
       <c r="H79" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="I79" t="n">
-        <v>20.0</v>
+        <v>13.0</v>
       </c>
       <c r="J79" t="n">
-        <v>9.0</v>
+        <v>14.0</v>
       </c>
       <c r="K79" t="n">
         <v>2.0</v>
       </c>
       <c r="L79" t="n">
-        <v>18.0</v>
+        <v>12.0</v>
       </c>
       <c r="M79" t="n">
-        <v>20.0</v>
+        <v>16.0</v>
       </c>
       <c r="N79" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="O79" t="n">
-        <v>17.0</v>
+        <v>6.0</v>
       </c>
       <c r="P79" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="Q79" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="80">
@@ -5419,49 +5419,49 @@
         <v>280</v>
       </c>
       <c r="C80" t="n">
-        <v>44.0</v>
+        <v>267.0</v>
       </c>
       <c r="D80" t="n">
-        <v>36.0</v>
+        <v>277.0</v>
       </c>
       <c r="E80" t="n">
-        <v>31.0</v>
+        <v>289.0</v>
       </c>
       <c r="F80" t="n">
-        <v>21.0</v>
+        <v>182.0</v>
       </c>
       <c r="G80" t="n">
-        <v>43.0</v>
+        <v>193.0</v>
       </c>
       <c r="H80" t="n">
-        <v>6.0</v>
+        <v>80.0</v>
       </c>
       <c r="I80" t="n">
-        <v>13.0</v>
+        <v>219.0</v>
       </c>
       <c r="J80" t="n">
-        <v>14.0</v>
+        <v>194.0</v>
       </c>
       <c r="K80" t="n">
-        <v>2.0</v>
+        <v>58.0</v>
       </c>
       <c r="L80" t="n">
-        <v>12.0</v>
+        <v>110.0</v>
       </c>
       <c r="M80" t="n">
-        <v>16.0</v>
+        <v>120.0</v>
       </c>
       <c r="N80" t="n">
-        <v>2.0</v>
+        <v>87.0</v>
       </c>
       <c r="O80" t="n">
-        <v>6.0</v>
+        <v>111.0</v>
       </c>
       <c r="P80" t="n">
-        <v>8.0</v>
+        <v>62.0</v>
       </c>
       <c r="Q80" t="n">
-        <v>8.0</v>
+        <v>228.0</v>
       </c>
     </row>
     <row r="81">

</xml_diff>